<commit_message>
Ajustei alguns elementos nos cards e nomenclaturas
</commit_message>
<xml_diff>
--- a/Indicadores Atração de Talentos.xlsx
+++ b/Indicadores Atração de Talentos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mongeralaegon-my.sharepoint.com/personal/roslima_mag_com_br/Documents/01. Projetos/Matriz de Indicadores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="8_{DD4BD1F1-0404-4DB3-9CDE-565CF2FC7490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E3950AA-7B36-44A0-A338-FE2953724D78}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{DD4BD1F1-0404-4DB3-9CDE-565CF2FC7490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E9C3D93-C10A-42DB-BC85-44F7F7666750}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B7F01D51-9716-43C2-8074-51E030286C40}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="70">
   <si>
     <t>Comercial: De todos que entram, quantos % começam a bater meta em X tempo (criar faixas de tempo), desconsiderando o tempo de formação.
 Corporativo: Ciclo de gente</t>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>Mede o ciclo de maturação do novo colaborador até atingir a performance plena. Essencial para o planejamento de headcount (definir quando contratar para atingir metas futuras) e para calcular o ROI das contratações, identificando o tempo necessário para que o profissional deixe de ser um custo operacional e passe a gerar retorno financeiro</t>
+  </si>
+  <si>
+    <t>MÉTRICA</t>
   </si>
 </sst>
 </file>
@@ -752,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798F919A-9319-42FB-8C23-79BA300CDE30}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:K11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,8 +838,8 @@
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="2:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>1</v>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>12</v>
@@ -865,8 +868,8 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>1</v>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>10</v>
@@ -896,7 +899,7 @@
     </row>
     <row r="6" spans="2:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>29</v>
@@ -958,7 +961,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1022,7 +1025,7 @@
     </row>
     <row r="10" spans="2:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>4</v>
@@ -1052,7 +1055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Ajustes no card de Candidado por vaga
</commit_message>
<xml_diff>
--- a/Indicadores Atração de Talentos.xlsx
+++ b/Indicadores Atração de Talentos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mongeralaegon-my.sharepoint.com/personal/roslima_mag_com_br/Documents/01. Projetos/Matriz de Indicadores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="8_{DD4BD1F1-0404-4DB3-9CDE-565CF2FC7490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E9C3D93-C10A-42DB-BC85-44F7F7666750}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="8_{DD4BD1F1-0404-4DB3-9CDE-565CF2FC7490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFE9B05E-90AD-44CF-BDB3-A02EEC75ED12}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B7F01D51-9716-43C2-8074-51E030286C40}"/>
   </bookViews>
@@ -267,7 +267,7 @@
     <t>Mede o ciclo de maturação do novo colaborador até atingir a performance plena. Essencial para o planejamento de headcount (definir quando contratar para atingir metas futuras) e para calcular o ROI das contratações, identificando o tempo necessário para que o profissional deixe de ser um custo operacional e passe a gerar retorno financeiro</t>
   </si>
   <si>
-    <t>MÉTRICA</t>
+    <t>Métrica</t>
   </si>
 </sst>
 </file>
@@ -756,7 +756,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Juste de nomenclatura dos cards
</commit_message>
<xml_diff>
--- a/Indicadores Atração de Talentos.xlsx
+++ b/Indicadores Atração de Talentos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mongeralaegon-my.sharepoint.com/personal/roslima_mag_com_br/Documents/01. Projetos/Matriz de Indicadores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="8_{DD4BD1F1-0404-4DB3-9CDE-565CF2FC7490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFE9B05E-90AD-44CF-BDB3-A02EEC75ED12}"/>
+  <xr:revisionPtr revIDLastSave="156" documentId="8_{DD4BD1F1-0404-4DB3-9CDE-565CF2FC7490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00DDA625-76C4-464E-9A2B-B74A583BAA26}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B7F01D51-9716-43C2-8074-51E030286C40}"/>
   </bookViews>
@@ -44,7 +44,7 @@
     <author>tc={F49FF4BF-5FC8-44C9-8C15-98E024937628}</author>
   </authors>
   <commentList>
-    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{F49FF4BF-5FC8-44C9-8C15-98E024937628}">
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{F49FF4BF-5FC8-44C9-8C15-98E024937628}">
       <text>
         <t>[Comentário encadeado]
 Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
@@ -69,15 +69,6 @@
     <t>Dimensionar por cargo.</t>
   </si>
   <si>
-    <t>Contratados diversos / contratados total</t>
-  </si>
-  <si>
-    <t>Taxa de diversidade na contratação</t>
-  </si>
-  <si>
-    <t>eNPS = % Promotores − % Detratores; Glassdoor = média das avaliações; Índice de reputação = média ponderada de notas em canais (Glassdoor, Indeed, Kununu) e menções positivas/negativas.</t>
-  </si>
-  <si>
     <t>Indice de Reputação</t>
   </si>
   <si>
@@ -87,15 +78,9 @@
     <t xml:space="preserve">Dimensionar por fonte. </t>
   </si>
   <si>
-    <t>Criar um fator que considere a Performance e o resultado da pesquisa de Fit Cultural.</t>
-  </si>
-  <si>
     <t>Qualidade da Contratação</t>
   </si>
   <si>
-    <t>desligados em 90 dias / efetivo do final do mês</t>
-  </si>
-  <si>
     <t>Taxa de saída em 90 dias</t>
   </si>
   <si>
@@ -135,9 +120,6 @@
     <t>Tipo</t>
   </si>
   <si>
-    <t>contratados permaneceu ≥6m / contratados totais.</t>
-  </si>
-  <si>
     <t>Efetivo</t>
   </si>
   <si>
@@ -147,93 +129,54 @@
     <t>Ponto focal a ser indicado pela Luciana</t>
   </si>
   <si>
-    <t>Número de candidatos por vaga</t>
-  </si>
-  <si>
-    <t>Taxa de Conversão por Etapa</t>
-  </si>
-  <si>
-    <t>Tempo total de seleção</t>
-  </si>
-  <si>
-    <t>Nº total de candidaturas recebidas / Nº de vagas abertas no período.</t>
-  </si>
-  <si>
     <t>Percentual de novos colaboradores que permanecem na companhia por pelo menos 180 dias. Este KPI ignora o turnover geral para focar especificamente na "curva de sobrevivência" inicial.</t>
   </si>
   <si>
     <t>Ciclo de Gente ou SGV / Pesquisa de Fit Cultural com a  Liderança</t>
   </si>
   <si>
-    <t>Avaliar se a integração (Onboarding) e o alinhamento de expectativas foram eficazes a médio prazo</t>
-  </si>
-  <si>
     <t>Mensal (com visão acumulada do semestre)</t>
   </si>
   <si>
     <t>Percentual de desligamentos (voluntários ou não) dentro do período de experiência.</t>
   </si>
   <si>
-    <t>Medir a eficácia do recrutamento e o "Fit Cultural". Erros aqui geram alto custo de recontratação imediata.</t>
-  </si>
-  <si>
     <t>Mensal</t>
   </si>
   <si>
     <t>Score que cruza dados de desempenho, atingimento de metas e adaptação cultural do novo colaborador.</t>
   </si>
   <si>
-    <t>Validar se o processo de seleção está trazendo os perfis que realmente geram valor ao negócio.</t>
-  </si>
-  <si>
     <t>Média de inscritos por posição aberta no período.</t>
   </si>
   <si>
     <t>Gupy</t>
   </si>
   <si>
-    <t>Medir a atratividade da marca empregadora e a assertividade dos canais de divulgação.</t>
-  </si>
-  <si>
     <t>Semestral (Exige tempo de maturação do desempenho)</t>
   </si>
   <si>
-    <t>% de candidatos por etapa do funil</t>
-  </si>
-  <si>
     <t>% de candidatos que avançam em cada fase do funil (candidatura → triagem → entrevista → oferta → contratação).</t>
   </si>
   <si>
     <t>Atração de Talentos</t>
   </si>
   <si>
-    <t>Identificar gargalos operacionais e etapas que estão "expulsando" bons talentos do processo.</t>
-  </si>
-  <si>
     <t>Dias corridos desde a abertura da requisição até o aceite da proposta pelo candidato.</t>
   </si>
   <si>
-    <t>data fechamento requisição − data_abertura</t>
-  </si>
-  <si>
     <t>Gupy/LG</t>
   </si>
   <si>
     <t>Atração de Talentos / Remuneração</t>
   </si>
   <si>
-    <t>Monitorar o SLA do RH e o impacto da "cadeira vazia" na produtividade das áreas.</t>
-  </si>
-  <si>
     <t>Monitoramento de notas e comentários em sites como Glassdoor e NPS de candidatos.</t>
   </si>
   <si>
     <t>Sistema de monitoramento da desses canais</t>
   </si>
   <si>
-    <t>Avaliar a percepção externa da empresa, o que impacta diretamente o custo de atração de talentos.</t>
-  </si>
-  <si>
     <t>Experiência do Colaborador?</t>
   </si>
   <si>
@@ -243,9 +186,6 @@
     <t>% de contratações de grupos minoritários em relação ao total de admissões.</t>
   </si>
   <si>
-    <t>Acompanhar o cumprimento de metas de ESG e promover um ambiente de inovação e inclusão.</t>
-  </si>
-  <si>
     <t>Produtividade do novo contratado (Ramp-up)</t>
   </si>
   <si>
@@ -258,9 +198,6 @@
     <t>SGV / Ciclo de Gente</t>
   </si>
   <si>
-    <t>Performance real do novo colaborador / Meta esperada para um colaborador pleno</t>
-  </si>
-  <si>
     <t>Planejamento Comercial / Experiência do Colaborador</t>
   </si>
   <si>
@@ -268,6 +205,76 @@
   </si>
   <si>
     <t>Métrica</t>
+  </si>
+  <si>
+    <t>Representa a consolidação do talento e o retorno do investimento inicial. Perder alguém nesta fase significa desperdiçar todo o custo de maturação e treinamento sem ter colhido os frutos da produtividade plena e autonomia do colaborador.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">É o termômetro crítico da Integração e do Alinhamento Cultural. Uma baixa retenção inicial indica que a promessa feita na contratação não condiz com a realidade, gerando altos custos de re-processamento e prejudicando o clima das equipes receptoras.
+</t>
+  </si>
+  <si>
+    <t>É o indicador que valida se o RH está entregando ativos de valor para o negócio. Contratações de alta qualidade elevam o patamar de entrega da companhia, reduzem a necessidade de gestão corretiva e aceleram o alcance das metas globais.</t>
+  </si>
+  <si>
+    <t>Criar um fator que considere a Performance e o resultado da pesquisa de Fit Cultural (Ex: (Desempenho Ciclo Gente + Nota de Alinhamento Cultural) / 2)</t>
+  </si>
+  <si>
+    <t>A marca empregadora funciona como um multiplicador de eficiência. Uma reputação sólida reduz o custo de aquisição de talentos e permite atrair perfis qualificados que priorizam cultura e propósito sobre remuneração.</t>
+  </si>
+  <si>
+    <t>Mede a saúde operacional do recrutamento. Gargalos em etapas específicas revelam processos burocráticos ou falta de calibração entre RH e gestores, o que aumenta o risco de perder excelentes candidatos por lentidão.</t>
+  </si>
+  <si>
+    <t>Mede o volume de interesse e a eficácia da estratégia de atração. Um alto índice (&gt;10) exige maior esforço de triagem técnica para focar na 'Concorrência Real', enquanto um baixo índice sinaliza desafios de remuneração ou employer branding. O equilíbrio garante critérios elevados sem sobrecarga operacional.</t>
+  </si>
+  <si>
+    <t>Tempo de Contratação</t>
+  </si>
+  <si>
+    <t>Representa o 'Custo da Cadeira Vazia'. Enquanto uma vaga crítica está aberta, há perda direta de receita, projetos atrasam e a equipe atual sofre sobrecarga, o que pode desencadear rotatividade por excesso de trabalho.</t>
+  </si>
+  <si>
+    <t>Diversidade é motor de inovação. Equipes plurais tomam decisões melhores, resolvem problemas complexos de forma mais criativa e garantem que os produtos da MAG reflitam a diversidade da nossa base de clientes.</t>
+  </si>
+  <si>
+    <t>Taxa de diversidade</t>
+  </si>
+  <si>
+    <t>% Grupos Minoritários (Candidatos vs Contratados)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Contratados permanentes &gt; 90 dias / Total Admissões)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Ativos com &gt; 6 meses / Total admissões há 6 meses)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Média Ponderada (Satisfação Interna + Glassdoor + Indeed)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Candidatos Aprovados / Candidatos Inscritos na Etapa)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Número Total de Candidatos Inscritos / Número de Vagas Disponíveis
+</t>
+  </si>
+  <si>
+    <t>Candidatos por vaga</t>
+  </si>
+  <si>
+    <t>Data de Aceite - Data de Abertura da Vaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dias até atingir 100% da Meta Esperada
+</t>
+  </si>
+  <si>
+    <t>Conversão por Etapa</t>
   </si>
 </sst>
 </file>
@@ -745,7 +752,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="H3" dT="2025-12-18T13:22:32.41" personId="{09A2FAA4-6A72-4E24-AACF-0106FA9FB2CC}" id="{F49FF4BF-5FC8-44C9-8C15-98E024937628}">
+  <threadedComment ref="H4" dT="2025-12-18T13:22:32.41" personId="{09A2FAA4-6A72-4E24-AACF-0106FA9FB2CC}" id="{F49FF4BF-5FC8-44C9-8C15-98E024937628}">
     <text>Luciana mencionou que está definindo pontos focais nos núcleos de Atração de Talentos e estes serão responsáveis pelo indicador do seu respectivo núcleo. Exemplo: Poliana responsável pelo Corporate.</text>
   </threadedComment>
 </ThreadedComments>
@@ -756,7 +763,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,220 +784,218 @@
     <row r="1" spans="2:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="I4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4" s="5"/>
     </row>
-    <row r="3" spans="2:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="5" t="s">
+    <row r="5" spans="2:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="5"/>
-    </row>
-    <row r="4" spans="2:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="2:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="H5" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="2:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="K6" s="3"/>
     </row>
     <row r="7" spans="2:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="G7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="45" x14ac:dyDescent="0.25">
@@ -998,58 +1003,60 @@
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="2:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>2</v>
@@ -1060,28 +1067,28 @@
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Ajustei o card para não mostrar os números
</commit_message>
<xml_diff>
--- a/Indicadores Atração de Talentos.xlsx
+++ b/Indicadores Atração de Talentos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mongeralaegon-my.sharepoint.com/personal/roslima_mag_com_br/Documents/01. Projetos/Matriz de Indicadores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="8_{DD4BD1F1-0404-4DB3-9CDE-565CF2FC7490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00DDA625-76C4-464E-9A2B-B74A583BAA26}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="8_{DD4BD1F1-0404-4DB3-9CDE-565CF2FC7490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{246AA178-268B-4C93-837A-BCD3C414BD80}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B7F01D51-9716-43C2-8074-51E030286C40}"/>
   </bookViews>
@@ -81,9 +81,6 @@
     <t>Qualidade da Contratação</t>
   </si>
   <si>
-    <t>Taxa de saída em 90 dias</t>
-  </si>
-  <si>
     <t>Trimestral</t>
   </si>
   <si>
@@ -275,23 +272,19 @@
   </si>
   <si>
     <t>Conversão por Etapa</t>
+  </si>
+  <si>
+    <t>Retenção 90 dias</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -386,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -397,20 +390,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -763,7 +753,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,123 +774,123 @@
     <row r="1" spans="2:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="J3" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="I4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="2:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>52</v>
+      <c r="D5" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K5" s="3"/>
     </row>
@@ -912,25 +902,25 @@
         <v>3</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="H6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K6" s="3"/>
     </row>
@@ -939,28 +929,28 @@
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="H7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>5</v>
@@ -968,31 +958,31 @@
     </row>
     <row r="8" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="G8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>5</v>
@@ -1003,28 +993,28 @@
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>4</v>
@@ -1032,31 +1022,31 @@
     </row>
     <row r="10" spans="2:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="I10" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>2</v>
@@ -1067,28 +1057,28 @@
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="3" t="s">
+      <c r="J11" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>0</v>

</xml_diff>